<commit_message>
Add brief readme and todo
</commit_message>
<xml_diff>
--- a/xls/FuncCov.xlsx
+++ b/xls/FuncCov.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fa58c1cc8ababdb2/Projects/VerifCoverage/VerifCov/xls/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fa58c1cc8ababdb2/Projects/VerifCoverage/xls/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="171" documentId="8_{080F2290-33DD-4D65-904E-390687414ED3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{32D0F004-20E6-40A8-8F2A-A7D0D78BFD6A}"/>
+  <xr:revisionPtr revIDLastSave="173" documentId="8_{080F2290-33DD-4D65-904E-390687414ED3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C7AB152B-BAE2-441F-BD86-99478212C8D5}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{D83558C4-0265-4DF9-9ACF-F20B1A7E37FC}"/>
   </bookViews>
@@ -707,12 +707,12 @@
   <dimension ref="A1:O28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.140625" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" customWidth="1"/>
     <col min="2" max="2" width="16.28515625" customWidth="1"/>
     <col min="3" max="3" width="18.5703125" customWidth="1"/>
     <col min="4" max="4" width="18.85546875" customWidth="1"/>

</xml_diff>